<commit_message>
looked at the newly downloaded species
</commit_message>
<xml_diff>
--- a/datasets/bird_species_new_add.xlsx
+++ b/datasets/bird_species_new_add.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dazedinthecity/Documents/GitHub/ceu-ds-project-groupB-2026/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B284EFA0-36A8-4A46-89DF-D31F38321890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B87D3C-417D-5B4E-AE0C-77AB20D07631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="2700" windowWidth="27640" windowHeight="16680" xr2:uid="{9B1C65BD-926B-4948-96E7-D8EAAD009C24}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="21460" xr2:uid="{9B1C65BD-926B-4948-96E7-D8EAAD009C24}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="59">
   <si>
     <t>eBird Code</t>
   </si>
@@ -139,9 +139,6 @@
     <t>Trend Summary</t>
   </si>
   <si>
-    <t>Unique Fact</t>
-  </si>
-  <si>
     <t>Red Knot</t>
   </si>
   <si>
@@ -190,9 +187,6 @@
     </r>
   </si>
   <si>
-    <t>In spring, they gather in the Wadden Sea by the hundreds of thousands, turning brick-red.</t>
-  </si>
-  <si>
     <t>Ruff</t>
   </si>
   <si>
@@ -213,9 +207,6 @@
     </r>
   </si>
   <si>
-    <t>Males have incredibly diverse "collars" of feathers used for mock-fighting during spring breaks.</t>
-  </si>
-  <si>
     <t>Garganey</t>
   </si>
   <si>
@@ -236,9 +227,6 @@
     </r>
   </si>
   <si>
-    <t>Known as the "Spring Teal" because it is one of the only ducks to winter entirely south of the Sahara.</t>
-  </si>
-  <si>
     <t>Wood Sandpiper</t>
   </si>
   <si>
@@ -257,9 +245,6 @@
       </rPr>
       <t xml:space="preserve"> One of the most common passage waders in inland European wetlands.</t>
     </r>
-  </si>
-  <si>
-    <t>They migrate in a broad front across the continent, often landing in tiny, temporary puddles.</t>
   </si>
   <si>
     <t>Osprey</t>
@@ -297,9 +282,6 @@
     </r>
   </si>
   <si>
-    <t>They are highly visible in spring as they follow major river systems (like the Rhine or Danube) North.</t>
-  </si>
-  <si>
     <t>Sanderling</t>
   </si>
   <si>
@@ -320,9 +302,6 @@
     </r>
   </si>
   <si>
-    <t>Famous for "running" like clockwork toys along the shoreline following the waves.</t>
-  </si>
-  <si>
     <t>Grey Plover</t>
   </si>
   <si>
@@ -343,13 +322,19 @@
     </r>
   </si>
   <si>
-    <t>Often called "Black-bellied Plovers" in spring when they molted into their striking tuxedo-like plumage.</t>
-  </si>
-  <si>
     <t>Bird Species (Spring migratory)</t>
   </si>
   <si>
     <t>Bird Species (Autumn migratory)</t>
+  </si>
+  <si>
+    <t>Migration Period</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>S</t>
   </si>
 </sst>
 </file>
@@ -743,292 +728,322 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{151FDC28-9546-154C-A49E-9C2B4DC35288}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="138" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="6" max="6" width="121.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="1" t="s">
+      <c r="C10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="C11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="1" t="s">
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="E12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F13" s="3" t="s">
+      <c r="F15" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="G15" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>